<commit_message>
scrie orele mai bine
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/FoaiePontaj.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/FoaiePontaj.xlsx
@@ -782,7 +782,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,14 +843,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,13 +875,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1"/>
@@ -1220,7 +1222,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1231,453 +1233,447 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BF38"/>
+  <dimension ref="A1:BE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="20" width="3" customWidth="1"/>
-    <col min="22" max="37" width="3" customWidth="1"/>
-    <col min="38" max="38" width="5.28515625" customWidth="1"/>
-    <col min="39" max="42" width="5.85546875" customWidth="1"/>
-    <col min="43" max="43" width="6.42578125" customWidth="1"/>
-    <col min="44" max="44" width="5.28515625" customWidth="1"/>
-    <col min="45" max="45" width="5.140625" customWidth="1"/>
-    <col min="46" max="58" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="19" width="3" customWidth="1"/>
+    <col min="21" max="36" width="3" customWidth="1"/>
+    <col min="37" max="37" width="5.28515625" customWidth="1"/>
+    <col min="38" max="41" width="5.85546875" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="44" max="44" width="5.140625" customWidth="1"/>
+    <col min="45" max="57" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="AI2" s="44" t="s">
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AH2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="AI3" s="44" t="s">
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AH3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AQ3" s="44" t="s">
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AP3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AR3" s="44"/>
-      <c r="AS3" s="44"/>
-      <c r="AT3" s="44"/>
-      <c r="AU3" s="44"/>
-      <c r="AV3" s="44"/>
-      <c r="AW3" s="44"/>
-      <c r="AX3" s="44"/>
-    </row>
-    <row r="4" spans="1:58" ht="15" x14ac:dyDescent="0.25">
-      <c r="S4" s="45" t="s">
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="37"/>
+    </row>
+    <row r="4" spans="1:57" ht="15" x14ac:dyDescent="0.25">
+      <c r="R4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AI4" s="44" t="s">
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AH4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AJ4" s="44"/>
-      <c r="AK4" s="44"/>
-      <c r="AL4" s="44"/>
-      <c r="AM4" s="44"/>
-      <c r="AN4" s="44"/>
-      <c r="AO4" s="44"/>
-      <c r="AQ4" s="44" t="s">
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+      <c r="AN4" s="37"/>
+      <c r="AP4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AR4" s="44"/>
-      <c r="AS4" s="44"/>
-      <c r="AT4" s="44"/>
-      <c r="AU4" s="44"/>
-      <c r="AV4" s="44"/>
-      <c r="AW4" s="44"/>
-      <c r="AX4" s="44"/>
-    </row>
-    <row r="5" spans="1:58" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="S5" s="46" t="s">
+      <c r="AQ4" s="37"/>
+      <c r="AR4" s="37"/>
+      <c r="AS4" s="37"/>
+      <c r="AT4" s="37"/>
+      <c r="AU4" s="37"/>
+      <c r="AV4" s="37"/>
+      <c r="AW4" s="37"/>
+    </row>
+    <row r="5" spans="1:57" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="R5" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AI5" s="44" t="s">
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="39"/>
+      <c r="AH5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="44"/>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
-      <c r="AN5" s="44"/>
-      <c r="AO5" s="44"/>
-      <c r="AQ5" s="44" t="s">
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="37"/>
+      <c r="AP5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="44"/>
-      <c r="AT5" s="44"/>
-      <c r="AU5" s="44"/>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="44"/>
-      <c r="AX5" s="44"/>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="AI6" s="44" t="s">
+      <c r="AQ5" s="37"/>
+      <c r="AR5" s="37"/>
+      <c r="AS5" s="37"/>
+      <c r="AT5" s="37"/>
+      <c r="AU5" s="37"/>
+      <c r="AV5" s="37"/>
+      <c r="AW5" s="37"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AH6" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AJ6" s="44"/>
-      <c r="AK6" s="44"/>
-      <c r="AL6" s="44"/>
-      <c r="AM6" s="44"/>
-      <c r="AN6" s="44"/>
-      <c r="AO6" s="44"/>
-      <c r="AQ6" s="44" t="s">
+      <c r="AI6" s="37"/>
+      <c r="AJ6" s="37"/>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="37"/>
+      <c r="AN6" s="37"/>
+      <c r="AP6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AR6" s="44"/>
-      <c r="AS6" s="44"/>
-      <c r="AT6" s="44"/>
-      <c r="AU6" s="44"/>
-      <c r="AV6" s="44"/>
-      <c r="AW6" s="44"/>
-      <c r="AX6" s="44"/>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="AI7" s="44" t="s">
+      <c r="AQ6" s="37"/>
+      <c r="AR6" s="37"/>
+      <c r="AS6" s="37"/>
+      <c r="AT6" s="37"/>
+      <c r="AU6" s="37"/>
+      <c r="AV6" s="37"/>
+      <c r="AW6" s="37"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AH7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AJ7" s="44"/>
-      <c r="AK7" s="44"/>
-      <c r="AL7" s="44"/>
-      <c r="AM7" s="44"/>
-      <c r="AN7" s="44"/>
-      <c r="AO7" s="44"/>
-      <c r="AQ7" s="44" t="s">
+      <c r="AI7" s="37"/>
+      <c r="AJ7" s="37"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="37"/>
+      <c r="AN7" s="37"/>
+      <c r="AP7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="44"/>
-      <c r="AT7" s="44"/>
-      <c r="AU7" s="44"/>
-      <c r="AV7" s="44"/>
-      <c r="AW7" s="44"/>
-      <c r="AX7" s="44"/>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="AI8" s="44" t="s">
+      <c r="AQ7" s="37"/>
+      <c r="AR7" s="37"/>
+      <c r="AS7" s="37"/>
+      <c r="AT7" s="37"/>
+      <c r="AU7" s="37"/>
+      <c r="AV7" s="37"/>
+      <c r="AW7" s="37"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="AH8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="AJ8" s="44"/>
-      <c r="AK8" s="44"/>
-      <c r="AL8" s="44"/>
-      <c r="AM8" s="44"/>
-      <c r="AN8" s="44"/>
-      <c r="AO8" s="44"/>
-      <c r="AQ8" s="44" t="s">
+      <c r="AI8" s="37"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="37"/>
+      <c r="AN8" s="37"/>
+      <c r="AP8" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="44"/>
-      <c r="AT8" s="44"/>
-      <c r="AU8" s="44"/>
-      <c r="AV8" s="44"/>
-      <c r="AW8" s="44"/>
-      <c r="AX8" s="44"/>
-    </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="AQ8" s="37"/>
+      <c r="AR8" s="37"/>
+      <c r="AS8" s="37"/>
+      <c r="AT8" s="37"/>
+      <c r="AU8" s="37"/>
+      <c r="AV8" s="37"/>
+      <c r="AW8" s="37"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
       <c r="E9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L9" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M9" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N9" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O9" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P9" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q9" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R9" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S9" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T9" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U9" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V9" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W9" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X9" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y9" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z9" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA9" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB9" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC9" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD9" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE9" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF9" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AG9" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH9" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI9" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AJ9" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AK9" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL9" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM9" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AN9" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AO9" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AP9" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AQ9" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AR9" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AS9" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AT9" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AU9" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AV9" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AW9" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AX9" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AY9" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AZ9" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BA9" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB9" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BC9" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BD9" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BE9" s="1">
-        <v>55</v>
-      </c>
-      <c r="BF9" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="6" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="E10" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="39"/>
-      <c r="AH10" s="39"/>
-      <c r="AI10" s="39"/>
-      <c r="AJ10" s="39"/>
-      <c r="AK10" s="40"/>
-      <c r="AL10" s="3" t="s">
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="41"/>
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="41"/>
+      <c r="AH10" s="41"/>
+      <c r="AI10" s="41"/>
+      <c r="AJ10" s="42"/>
+      <c r="AK10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AM10" s="38" t="s">
+      <c r="AL10" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="39"/>
-      <c r="AP10" s="39"/>
-      <c r="AQ10" s="40"/>
-      <c r="AR10" s="3" t="s">
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AS10" s="14" t="s">
+      <c r="AR10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AT10" s="38" t="s">
+      <c r="AS10" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="AU10" s="39"/>
-      <c r="AV10" s="39"/>
-      <c r="AW10" s="39"/>
-      <c r="AX10" s="39"/>
-      <c r="AY10" s="39"/>
-      <c r="AZ10" s="39"/>
-      <c r="BA10" s="39"/>
-      <c r="BB10" s="39"/>
-      <c r="BC10" s="39"/>
-      <c r="BD10" s="39"/>
-      <c r="BE10" s="39"/>
-      <c r="BF10" s="40"/>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="AT10" s="41"/>
+      <c r="AU10" s="41"/>
+      <c r="AV10" s="41"/>
+      <c r="AW10" s="41"/>
+      <c r="AX10" s="41"/>
+      <c r="AY10" s="41"/>
+      <c r="AZ10" s="41"/>
+      <c r="BA10" s="41"/>
+      <c r="BB10" s="41"/>
+      <c r="BC10" s="41"/>
+      <c r="BD10" s="41"/>
+      <c r="BE10" s="42"/>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1685,176 +1681,177 @@
         <v>20</v>
       </c>
       <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="42"/>
-      <c r="AA11" s="42"/>
-      <c r="AB11" s="42"/>
-      <c r="AC11" s="42"/>
-      <c r="AD11" s="42"/>
-      <c r="AE11" s="42"/>
-      <c r="AF11" s="42"/>
-      <c r="AG11" s="42"/>
-      <c r="AH11" s="42"/>
-      <c r="AI11" s="42"/>
-      <c r="AJ11" s="42"/>
-      <c r="AK11" s="43"/>
-      <c r="AL11" s="4" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="44"/>
+      <c r="X11" s="44"/>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="44"/>
+      <c r="AA11" s="44"/>
+      <c r="AB11" s="44"/>
+      <c r="AC11" s="44"/>
+      <c r="AD11" s="44"/>
+      <c r="AE11" s="44"/>
+      <c r="AF11" s="44"/>
+      <c r="AG11" s="44"/>
+      <c r="AH11" s="44"/>
+      <c r="AI11" s="44"/>
+      <c r="AJ11" s="45"/>
+      <c r="AK11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AM11" s="32"/>
-      <c r="AN11" s="33"/>
-      <c r="AO11" s="33"/>
-      <c r="AP11" s="33"/>
-      <c r="AQ11" s="34"/>
-      <c r="AR11" s="4" t="s">
+      <c r="AL11" s="46"/>
+      <c r="AM11" s="47"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="47"/>
+      <c r="AP11" s="48"/>
+      <c r="AQ11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AS11" s="13" t="s">
+      <c r="AR11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AT11" s="32"/>
-      <c r="AU11" s="33"/>
-      <c r="AV11" s="33"/>
-      <c r="AW11" s="33"/>
-      <c r="AX11" s="33"/>
-      <c r="AY11" s="33"/>
-      <c r="AZ11" s="33"/>
-      <c r="BA11" s="33"/>
-      <c r="BB11" s="33"/>
-      <c r="BC11" s="33"/>
-      <c r="BD11" s="33"/>
-      <c r="BE11" s="33"/>
-      <c r="BF11" s="34"/>
-    </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="AS11" s="46"/>
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="47"/>
+      <c r="AW11" s="47"/>
+      <c r="AX11" s="47"/>
+      <c r="AY11" s="47"/>
+      <c r="AZ11" s="47"/>
+      <c r="BA11" s="47"/>
+      <c r="BB11" s="47"/>
+      <c r="BC11" s="47"/>
+      <c r="BD11" s="47"/>
+      <c r="BE11" s="48"/>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9">
+      <c r="D12" s="7"/>
+      <c r="E12" s="9">
         <v>1</v>
       </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
       <c r="G12" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" s="6">
-        <v>3</v>
-      </c>
-      <c r="I12" s="6">
         <v>4</v>
       </c>
+      <c r="I12" s="12">
+        <v>5</v>
+      </c>
       <c r="J12" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K12" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L12" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M12" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N12" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P12" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q12" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R12" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S12" s="12">
-        <v>14</v>
-      </c>
-      <c r="T12" s="12">
         <v>15</v>
       </c>
-      <c r="U12" s="14" t="s">
+      <c r="T12" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="U12" s="12">
+        <v>16</v>
+      </c>
       <c r="V12" s="12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="W12" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="X12" s="12">
+        <v>19</v>
+      </c>
+      <c r="Y12" s="12">
+        <v>20</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>21</v>
+      </c>
+      <c r="AA12" s="12">
+        <v>22</v>
+      </c>
+      <c r="AB12" s="12">
+        <v>23</v>
+      </c>
+      <c r="AC12" s="12">
+        <v>24</v>
+      </c>
+      <c r="AD12" s="12">
+        <v>25</v>
+      </c>
+      <c r="AE12" s="12">
+        <v>26</v>
+      </c>
+      <c r="AF12" s="12">
+        <v>27</v>
+      </c>
+      <c r="AG12" s="12">
+        <v>28</v>
+      </c>
+      <c r="AH12" s="12">
+        <v>29</v>
+      </c>
+      <c r="AI12" s="12">
+        <v>30</v>
+      </c>
+      <c r="AJ12" s="12">
+        <v>31</v>
+      </c>
+      <c r="AK12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="12">
-        <v>19</v>
-      </c>
-      <c r="Z12" s="12">
-        <v>20</v>
-      </c>
-      <c r="AA12" s="12">
-        <v>21</v>
-      </c>
-      <c r="AB12" s="12">
-        <v>22</v>
-      </c>
-      <c r="AC12" s="12">
-        <v>23</v>
-      </c>
-      <c r="AD12" s="12">
-        <v>24</v>
-      </c>
-      <c r="AE12" s="12">
-        <v>25</v>
-      </c>
-      <c r="AF12" s="12">
-        <v>26</v>
-      </c>
-      <c r="AG12" s="12">
-        <v>27</v>
-      </c>
-      <c r="AH12" s="12">
-        <v>28</v>
-      </c>
-      <c r="AI12" s="12">
-        <v>29</v>
-      </c>
-      <c r="AJ12" s="12">
-        <v>30</v>
-      </c>
-      <c r="AK12" s="12">
-        <v>31</v>
-      </c>
-      <c r="AL12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM12" s="3" t="s">
+      <c r="AM12" s="14" t="s">
         <v>18</v>
       </c>
       <c r="AN12" s="14" t="s">
@@ -1866,65 +1863,62 @@
       <c r="AP12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AQ12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR12" s="4" t="s">
+      <c r="AQ12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AS12" s="13" t="s">
+      <c r="AR12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AT12" s="18" t="s">
+      <c r="AS12" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="AT12" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="AU12" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AV12" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AW12" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AX12" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AY12" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ12" s="19" t="s">
         <v>27</v>
       </c>
+      <c r="AZ12" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="BA12" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB12" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BC12" s="20" t="s">
         <v>35</v>
       </c>
       <c r="BD12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="BE12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="BF12" s="22" t="s">
+      <c r="BE12" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -1935,10 +1929,10 @@
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
       <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="15" t="s">
+      <c r="T13" s="15" t="s">
         <v>37</v>
       </c>
+      <c r="U13" s="13"/>
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
@@ -1954,9 +1948,11 @@
       <c r="AH13" s="13"/>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="4" t="s">
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM13" s="13" t="s">
         <v>38</v>
       </c>
       <c r="AN13" s="13" t="s">
@@ -1966,51 +1962,48 @@
         <v>38</v>
       </c>
       <c r="AP13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AR13" s="4"/>
-      <c r="AS13" s="13" t="s">
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AT13" s="21" t="s">
+      <c r="AS13" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="AT13" s="22"/>
       <c r="AU13" s="22"/>
       <c r="AV13" s="22"/>
-      <c r="AW13" s="22"/>
-      <c r="AX13" s="22" t="s">
+      <c r="AW13" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="AX13" s="22"/>
       <c r="AY13" s="22"/>
-      <c r="AZ13" s="22"/>
+      <c r="AZ13" s="20"/>
       <c r="BA13" s="20"/>
-      <c r="BB13" s="20"/>
+      <c r="BB13" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="BC13" s="20" t="s">
         <v>43</v>
       </c>
       <c r="BD13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="BE13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="BF13" s="22" t="s">
+      <c r="BE13" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="11"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2038,49 +2031,48 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="5"/>
-      <c r="AM14" s="16">
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="16">
         <v>2</v>
       </c>
+      <c r="AM14" s="17">
+        <v>1.75</v>
+      </c>
       <c r="AN14" s="17">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="AO14" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="AP14" s="17">
         <v>1</v>
       </c>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="5"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="23" t="s">
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="23" t="s">
         <v>46</v>
       </c>
+      <c r="AT14" s="24"/>
       <c r="AU14" s="24"/>
       <c r="AV14" s="24"/>
       <c r="AW14" s="24"/>
       <c r="AX14" s="24"/>
       <c r="AY14" s="24"/>
-      <c r="AZ14" s="24"/>
+      <c r="AZ14" s="25"/>
       <c r="BA14" s="25"/>
-      <c r="BB14" s="25"/>
+      <c r="BB14" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="BC14" s="26" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="BD14" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="BE14" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="BF14" s="24"/>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="BE14" s="24"/>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
@@ -2135,12 +2127,8 @@
       <c r="BC15" s="27"/>
       <c r="BD15" s="27"/>
       <c r="BE15" s="27"/>
-      <c r="BF15" s="27"/>
-    </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+    </row>
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
@@ -2195,12 +2183,8 @@
       <c r="BC16" s="28"/>
       <c r="BD16" s="28"/>
       <c r="BE16" s="28"/>
-      <c r="BF16" s="28"/>
-    </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+    </row>
+    <row r="17" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
@@ -2255,12 +2239,8 @@
       <c r="BC17" s="28"/>
       <c r="BD17" s="28"/>
       <c r="BE17" s="28"/>
-      <c r="BF17" s="28"/>
-    </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+    </row>
+    <row r="18" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
@@ -2315,12 +2295,8 @@
       <c r="BC18" s="28"/>
       <c r="BD18" s="28"/>
       <c r="BE18" s="28"/>
-      <c r="BF18" s="28"/>
-    </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+    </row>
+    <row r="19" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
@@ -2375,12 +2351,8 @@
       <c r="BC19" s="28"/>
       <c r="BD19" s="28"/>
       <c r="BE19" s="28"/>
-      <c r="BF19" s="28"/>
-    </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+    </row>
+    <row r="20" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
@@ -2435,12 +2407,8 @@
       <c r="BC20" s="28"/>
       <c r="BD20" s="28"/>
       <c r="BE20" s="28"/>
-      <c r="BF20" s="28"/>
-    </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+    </row>
+    <row r="21" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
@@ -2495,12 +2463,8 @@
       <c r="BC21" s="28"/>
       <c r="BD21" s="28"/>
       <c r="BE21" s="28"/>
-      <c r="BF21" s="28"/>
-    </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+    </row>
+    <row r="22" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
@@ -2555,12 +2519,8 @@
       <c r="BC22" s="28"/>
       <c r="BD22" s="28"/>
       <c r="BE22" s="28"/>
-      <c r="BF22" s="28"/>
-    </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+    </row>
+    <row r="23" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
@@ -2615,12 +2575,8 @@
       <c r="BC23" s="28"/>
       <c r="BD23" s="28"/>
       <c r="BE23" s="28"/>
-      <c r="BF23" s="28"/>
-    </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+    </row>
+    <row r="24" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
@@ -2675,12 +2631,8 @@
       <c r="BC24" s="28"/>
       <c r="BD24" s="28"/>
       <c r="BE24" s="28"/>
-      <c r="BF24" s="28"/>
-    </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+    </row>
+    <row r="25" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
@@ -2735,12 +2687,8 @@
       <c r="BC25" s="28"/>
       <c r="BD25" s="28"/>
       <c r="BE25" s="28"/>
-      <c r="BF25" s="28"/>
-    </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+    </row>
+    <row r="26" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
@@ -2795,12 +2743,8 @@
       <c r="BC26" s="28"/>
       <c r="BD26" s="28"/>
       <c r="BE26" s="28"/>
-      <c r="BF26" s="28"/>
-    </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+    </row>
+    <row r="27" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
@@ -2855,12 +2799,8 @@
       <c r="BC27" s="28"/>
       <c r="BD27" s="28"/>
       <c r="BE27" s="28"/>
-      <c r="BF27" s="28"/>
-    </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+    </row>
+    <row r="28" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
@@ -2915,12 +2855,8 @@
       <c r="BC28" s="28"/>
       <c r="BD28" s="28"/>
       <c r="BE28" s="28"/>
-      <c r="BF28" s="28"/>
-    </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+    </row>
+    <row r="29" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
@@ -2975,12 +2911,8 @@
       <c r="BC29" s="28"/>
       <c r="BD29" s="28"/>
       <c r="BE29" s="28"/>
-      <c r="BF29" s="28"/>
-    </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+    </row>
+    <row r="30" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
@@ -3035,12 +2967,8 @@
       <c r="BC30" s="28"/>
       <c r="BD30" s="28"/>
       <c r="BE30" s="28"/>
-      <c r="BF30" s="28"/>
-    </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+    </row>
+    <row r="31" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
@@ -3095,12 +3023,8 @@
       <c r="BC31" s="28"/>
       <c r="BD31" s="28"/>
       <c r="BE31" s="28"/>
-      <c r="BF31" s="28"/>
-    </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+    </row>
+    <row r="32" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
@@ -3155,12 +3079,8 @@
       <c r="BC32" s="28"/>
       <c r="BD32" s="28"/>
       <c r="BE32" s="28"/>
-      <c r="BF32" s="28"/>
-    </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+    </row>
+    <row r="33" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
@@ -3215,12 +3135,8 @@
       <c r="BC33" s="28"/>
       <c r="BD33" s="28"/>
       <c r="BE33" s="28"/>
-      <c r="BF33" s="28"/>
-    </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+    </row>
+    <row r="34" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
@@ -3275,12 +3191,8 @@
       <c r="BC34" s="28"/>
       <c r="BD34" s="28"/>
       <c r="BE34" s="28"/>
-      <c r="BF34" s="28"/>
-    </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+    </row>
+    <row r="35" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -3335,12 +3247,8 @@
       <c r="BC35" s="28"/>
       <c r="BD35" s="28"/>
       <c r="BE35" s="28"/>
-      <c r="BF35" s="28"/>
-    </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+    </row>
+    <row r="36" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
@@ -3395,12 +3303,8 @@
       <c r="BC36" s="28"/>
       <c r="BD36" s="28"/>
       <c r="BE36" s="28"/>
-      <c r="BF36" s="28"/>
-    </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
+    </row>
+    <row r="37" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -3455,12 +3359,8 @@
       <c r="BC37" s="28"/>
       <c r="BD37" s="28"/>
       <c r="BE37" s="28"/>
-      <c r="BF37" s="28"/>
-    </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
+    </row>
+    <row r="38" spans="4:57" x14ac:dyDescent="0.2">
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
@@ -3515,37 +3415,30 @@
       <c r="BC38" s="28"/>
       <c r="BD38" s="28"/>
       <c r="BE38" s="28"/>
-      <c r="BF38" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="S4:AD4"/>
-    <mergeCell ref="S5:AD5"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AI3:AO3"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AI5:AO5"/>
-    <mergeCell ref="AI6:AO6"/>
-    <mergeCell ref="AI7:AO7"/>
-    <mergeCell ref="AI8:AO8"/>
-    <mergeCell ref="AQ3:AX3"/>
-    <mergeCell ref="AQ4:AX4"/>
-    <mergeCell ref="AQ5:AX5"/>
-    <mergeCell ref="AQ6:AX6"/>
-    <mergeCell ref="AQ7:AX7"/>
-    <mergeCell ref="AQ8:AX8"/>
-    <mergeCell ref="AM10:AQ10"/>
-    <mergeCell ref="AT10:BF10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="F11:AK11"/>
-    <mergeCell ref="AM11:AQ11"/>
-    <mergeCell ref="AT11:BF11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="F10:AK10"/>
+  <mergeCells count="21">
+    <mergeCell ref="E10:AJ10"/>
+    <mergeCell ref="AL10:AP10"/>
+    <mergeCell ref="AS10:BE10"/>
+    <mergeCell ref="E11:AJ11"/>
+    <mergeCell ref="AL11:AP11"/>
+    <mergeCell ref="AS11:BE11"/>
+    <mergeCell ref="AH6:AN6"/>
+    <mergeCell ref="AH7:AN7"/>
+    <mergeCell ref="AH8:AN8"/>
+    <mergeCell ref="AP3:AW3"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AP5:AW5"/>
+    <mergeCell ref="AP6:AW6"/>
+    <mergeCell ref="AP7:AW7"/>
+    <mergeCell ref="AP8:AW8"/>
+    <mergeCell ref="R4:AC4"/>
+    <mergeCell ref="R5:AC5"/>
+    <mergeCell ref="AH2:AN2"/>
+    <mergeCell ref="AH3:AN3"/>
+    <mergeCell ref="AH4:AN4"/>
+    <mergeCell ref="AH5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>